<commit_message>
2022.4.5-1 rgb img fix
</commit_message>
<xml_diff>
--- a/src/Temp/JsonWorker/Collect/【特征对照表】.xlsx
+++ b/src/Temp/JsonWorker/Collect/【特征对照表】.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="12995"/>
+    <workbookView windowWidth="16991" windowHeight="13595"/>
   </bookViews>
   <sheets>
     <sheet name="有码" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="868">
   <si>
     <t>JavDb</t>
   </si>
@@ -2614,6 +2614,9 @@
   </si>
   <si>
     <t>女優手淫</t>
+  </si>
+  <si>
+    <t>高跟鞋</t>
   </si>
   <si>
     <t>重新整理</t>
@@ -2624,9 +2627,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -2647,9 +2650,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2660,9 +2671,93 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2684,86 +2779,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2771,20 +2788,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2799,7 +2802,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2811,13 +2964,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2829,157 +2976,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2990,17 +2993,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -3015,45 +3007,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3082,6 +3035,56 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -3096,10 +3099,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3108,133 +3111,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3611,12 +3614,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G414"/>
+  <dimension ref="A1:G415"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A387" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E96" sqref="E96"/>
+      <selection pane="bottomLeft" activeCell="E415" sqref="E415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -10144,6 +10147,20 @@
       </c>
       <c r="F414" s="3" t="s">
         <v>332</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6">
+      <c r="A415" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="D415" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="E415" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="F415" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -10174,7 +10191,7 @@
         <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C1" t="s">
         <v>440</v>

</xml_diff>